<commit_message>
Inclusao da distancia entre apoios
</commit_message>
<xml_diff>
--- a/app.xlsx
+++ b/app.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02 - Ulisses\Cursos\Python\Mec Sol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02 - Ulisses\Cursos\Python\Momentos_Mec_Sol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAF753B9-BC29-4B31-9F6C-C6845DB73698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C89CE3-E7B8-4E0C-A6FA-795527CE2B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B81118AB-4249-4E54-B3FF-127817C07719}"/>
+    <workbookView xWindow="-21720" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{B81118AB-4249-4E54-B3FF-127817C07719}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Sobre</t>
   </si>
@@ -59,12 +59,6 @@
     <t>Q (KN)</t>
   </si>
   <si>
-    <t>Início</t>
-  </si>
-  <si>
-    <t>Fim</t>
-  </si>
-  <si>
     <t>Calcular</t>
   </si>
   <si>
@@ -77,16 +71,57 @@
     <t>Sair</t>
   </si>
   <si>
-    <t>Q (KN/m)</t>
+    <t>Distancia entre os pontos de apoio em metros</t>
+  </si>
+  <si>
+    <t>Distancia (m):</t>
+  </si>
+  <si>
+    <t>Carga 1:</t>
+  </si>
+  <si>
+    <t>Carga 2:</t>
+  </si>
+  <si>
+    <t>Carga 3:</t>
+  </si>
+  <si>
+    <t>Carga 4:</t>
+  </si>
+  <si>
+    <t>Carga 5:</t>
+  </si>
+  <si>
+    <t>Q (KN/m):</t>
+  </si>
+  <si>
+    <t>Início:</t>
+  </si>
+  <si>
+    <t>Fim:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -193,13 +228,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -207,13 +241,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACBD08E-DE45-41EC-AF92-D7180A1EA36F}">
-  <dimension ref="D2:I24"/>
+  <dimension ref="D2:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,223 +592,182 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
       <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="13" t="s">
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="4">
-        <v>3</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
+      <c r="I12" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="4">
-        <v>4</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="4">
-        <v>5</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6" t="s">
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="6"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="9"/>
+      <c r="D24" s="4"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="4"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D12:I12"/>
+  <mergeCells count="6">
+    <mergeCell ref="D14:I14"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Remoção da coordenada Y
Para os calculos, não são necessárias as coordenadas Y das cargas. O usuário deverá fornecer apenas a coordenada X

Tratamento de erro para valores de X maiores que o tamanho da viga e inferiores a zero, pois caracterizam cargas fora da viga.
</commit_message>
<xml_diff>
--- a/app.xlsx
+++ b/app.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02 - Ulisses\Cursos\Python\Momentos_Mec_Sol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C89CE3-E7B8-4E0C-A6FA-795527CE2B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402D2B27-EE13-4929-B2F2-ECDD2F601B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{B81118AB-4249-4E54-B3FF-127817C07719}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Sobre</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Fim:</t>
+  </si>
+  <si>
+    <t>Coluna y removida</t>
   </si>
 </sst>
 </file>
@@ -128,13 +131,19 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -228,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -238,6 +247,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,15 +265,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,15 +583,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACBD08E-DE45-41EC-AF92-D7180A1EA36F}">
-  <dimension ref="D2:I26"/>
+  <dimension ref="D2:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,29 +601,32 @@
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="9" t="s">
+    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D4" s="9" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
       <c r="E5" t="s">
         <v>6</v>
@@ -621,66 +634,71 @@
       <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="16" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="G6" s="16"/>
       <c r="H6" t="s">
         <v>18</v>
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="G7" s="16"/>
       <c r="H7" t="s">
         <v>19</v>
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="G8" s="16"/>
       <c r="H8" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G9" s="16"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="G10" s="16"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="12" t="s">
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="15" t="s">
+    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
       <c r="H12" t="s">
         <v>7</v>
       </c>
@@ -688,31 +706,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="9" t="s">
+    <row r="13" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="9" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
       <c r="I16" s="5"/>
     </row>

</xml_diff>

<commit_message>
Exibe e oculta cargas pontuais
Criadas funcoes que desabilitam a entrada de novos valores enquanto nao for solicitado pelo usuario

Inserido botoes que permitem exibir e ocultar as cargas pontuais e as cargas distribuidas
</commit_message>
<xml_diff>
--- a/app.xlsx
+++ b/app.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02 - Ulisses\Cursos\Python\Momentos_Mec_Sol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402D2B27-EE13-4929-B2F2-ECDD2F601B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09AA986-7460-4B01-8262-83A2C2FE84A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{B81118AB-4249-4E54-B3FF-127817C07719}"/>
+    <workbookView xWindow="-23820" yWindow="945" windowWidth="21600" windowHeight="11385" xr2:uid="{B81118AB-4249-4E54-B3FF-127817C07719}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Sobre</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Coluna y removida</t>
+  </si>
+  <si>
+    <t>Cargas Pontuais</t>
+  </si>
+  <si>
+    <t>Cargas Distribuidas</t>
   </si>
 </sst>
 </file>
@@ -237,38 +243,72 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,13 +623,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACBD08E-DE45-41EC-AF92-D7180A1EA36F}">
-  <dimension ref="D2:M26"/>
+  <dimension ref="C2:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
@@ -602,29 +647,29 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="19"/>
       <c r="M3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="13"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
@@ -634,7 +679,7 @@
       <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="5"/>
@@ -643,7 +688,7 @@
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="8"/>
       <c r="H6" t="s">
         <v>18</v>
       </c>
@@ -653,7 +698,7 @@
       <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="16"/>
+      <c r="G7" s="8"/>
       <c r="H7" t="s">
         <v>19</v>
       </c>
@@ -663,7 +708,7 @@
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="16"/>
+      <c r="G8" s="8"/>
       <c r="H8" t="s">
         <v>20</v>
       </c>
@@ -673,14 +718,14 @@
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="16"/>
+      <c r="G9" s="8"/>
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="8"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="4:13" x14ac:dyDescent="0.25">
@@ -693,7 +738,7 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="9"/>
@@ -707,85 +752,275 @@
       </c>
     </row>
     <row r="13" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D15" s="4"/>
-      <c r="I15" s="5"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D16" s="4"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="4"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="4"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="4"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="24"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>3</v>
+      </c>
       <c r="D20" s="4"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D21" s="4"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="4"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="4"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="4"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="4"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="8"/>
+      <c r="E20" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="22"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="22"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="11"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="D28:I28"/>
     <mergeCell ref="D14:I14"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D13:I13"/>
     <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="J17:K26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>